<commit_message>
Actualizacion de horarios del GANTT Terminado
</commit_message>
<xml_diff>
--- a/GANTT.xlsx
+++ b/GANTT.xlsx
@@ -38,9 +38,6 @@
     <t>Nombre Actividad</t>
   </si>
   <si>
-    <t>Creación de Git</t>
-  </si>
-  <si>
     <t>CPM Y  Gantt</t>
   </si>
   <si>
@@ -50,9 +47,6 @@
     <t>DER</t>
   </si>
   <si>
-    <t>Diagrama de Clases</t>
-  </si>
-  <si>
     <t>Creación BDD</t>
   </si>
   <si>
@@ -78,6 +72,12 @@
   </si>
   <si>
     <t xml:space="preserve">Carpetas de campo completas </t>
+  </si>
+  <si>
+    <t>Diagrama de Clases (UML)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Creación de Git </t>
   </si>
 </sst>
 </file>
@@ -100,7 +100,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -122,6 +122,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -153,14 +165,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -205,6 +211,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -486,10 +507,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:P17"/>
+  <dimension ref="B1:U17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" zoomScale="148" zoomScaleNormal="148" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -497,343 +518,575 @@
     <col min="1" max="1" width="4.28515625" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" customWidth="1"/>
     <col min="3" max="3" width="45.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.28515625" customWidth="1"/>
-    <col min="7" max="7" width="5.5703125" customWidth="1"/>
-    <col min="8" max="8" width="5.140625" customWidth="1"/>
-    <col min="9" max="10" width="6" customWidth="1"/>
-    <col min="11" max="11" width="6.140625" customWidth="1"/>
-    <col min="12" max="12" width="5.42578125" customWidth="1"/>
-    <col min="13" max="13" width="5.85546875" customWidth="1"/>
-    <col min="14" max="14" width="5.42578125" customWidth="1"/>
-    <col min="15" max="15" width="5.28515625" customWidth="1"/>
-    <col min="16" max="16" width="5.85546875" customWidth="1"/>
+    <col min="6" max="6" width="4.7109375" customWidth="1"/>
+    <col min="7" max="7" width="4.28515625" customWidth="1"/>
+    <col min="8" max="8" width="4.85546875" customWidth="1"/>
+    <col min="9" max="13" width="5.28515625" customWidth="1"/>
+    <col min="14" max="14" width="6" customWidth="1"/>
+    <col min="15" max="15" width="6.140625" customWidth="1"/>
+    <col min="16" max="16" width="5.42578125" customWidth="1"/>
+    <col min="17" max="17" width="5.85546875" customWidth="1"/>
+    <col min="18" max="18" width="5.42578125" customWidth="1"/>
+    <col min="19" max="19" width="5.28515625" customWidth="1"/>
+    <col min="20" max="20" width="5.85546875" customWidth="1"/>
+    <col min="21" max="21" width="5.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:16" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="3" t="s">
+    <row r="1" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="F1" s="20">
+        <v>1</v>
+      </c>
+      <c r="G1" s="20">
+        <v>2</v>
+      </c>
+      <c r="H1" s="20">
+        <v>3</v>
+      </c>
+      <c r="I1" s="20">
+        <v>4</v>
+      </c>
+      <c r="J1" s="20">
+        <v>5</v>
+      </c>
+      <c r="K1" s="20">
+        <v>6</v>
+      </c>
+      <c r="L1" s="20">
+        <v>7</v>
+      </c>
+      <c r="M1" s="20">
+        <v>8</v>
+      </c>
+      <c r="N1" s="20">
+        <v>9</v>
+      </c>
+      <c r="O1" s="20">
+        <v>10</v>
+      </c>
+      <c r="P1" s="20">
+        <v>11</v>
+      </c>
+      <c r="Q1" s="20">
+        <v>12</v>
+      </c>
+      <c r="R1" s="20">
+        <v>13</v>
+      </c>
+      <c r="S1" s="20">
+        <v>14</v>
+      </c>
+      <c r="T1" s="20">
+        <v>15</v>
+      </c>
+      <c r="U1" s="20">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="2:21" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2" s="3">
         <v>44855</v>
       </c>
-      <c r="G2" s="5">
+      <c r="G2" s="3">
         <v>44858</v>
       </c>
-      <c r="H2" s="5">
+      <c r="H2" s="3">
+        <v>44861</v>
+      </c>
+      <c r="I2" s="3">
         <v>44862</v>
       </c>
-      <c r="I2" s="5">
+      <c r="J2" s="3">
         <v>44865</v>
       </c>
-      <c r="J2" s="5">
+      <c r="K2" s="3">
+        <v>44868</v>
+      </c>
+      <c r="L2" s="3">
         <v>44869</v>
       </c>
-      <c r="K2" s="5">
+      <c r="M2" s="3">
         <v>44872</v>
       </c>
-      <c r="L2" s="5">
+      <c r="N2" s="3">
+        <v>44875</v>
+      </c>
+      <c r="O2" s="3">
         <v>44876</v>
       </c>
-      <c r="M2" s="5">
+      <c r="P2" s="3">
         <v>44879</v>
       </c>
-      <c r="N2" s="5">
+      <c r="Q2" s="3">
+        <v>44882</v>
+      </c>
+      <c r="R2" s="3">
         <v>44883</v>
       </c>
-      <c r="O2" s="1"/>
-      <c r="P2" s="2"/>
-    </row>
-    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B3" s="6">
+      <c r="S2" s="3">
+        <v>44886</v>
+      </c>
+      <c r="T2" s="3">
+        <v>44889</v>
+      </c>
+      <c r="U2" s="3">
+        <v>44890</v>
+      </c>
+    </row>
+    <row r="3" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B3" s="4">
         <v>1</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="19">
+        <v>44855</v>
+      </c>
+      <c r="E3" s="19">
+        <v>44858</v>
+      </c>
+      <c r="F3" s="18"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="14"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4"/>
+      <c r="Q3" s="4"/>
+      <c r="R3" s="4"/>
+      <c r="S3" s="14"/>
+      <c r="T3" s="14"/>
+      <c r="U3" s="14"/>
+    </row>
+    <row r="4" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B4" s="4">
+        <v>2</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
-    </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B4" s="6">
-        <v>2</v>
-      </c>
-      <c r="C4" s="6" t="s">
+      <c r="D4" s="19">
+        <v>44858</v>
+      </c>
+      <c r="E4" s="19">
+        <v>44861</v>
+      </c>
+      <c r="F4" s="18"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="4"/>
+      <c r="R4" s="4"/>
+      <c r="S4" s="14"/>
+      <c r="T4" s="14"/>
+      <c r="U4" s="14"/>
+    </row>
+    <row r="5" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B5" s="4">
+        <v>3</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
-      <c r="N4" s="6"/>
-    </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B5" s="6">
-        <v>3</v>
-      </c>
-      <c r="C5" s="6" t="s">
+      <c r="D5" s="19">
+        <v>44861</v>
+      </c>
+      <c r="E5" s="19">
+        <v>44862</v>
+      </c>
+      <c r="F5" s="4"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="4"/>
+      <c r="Q5" s="4"/>
+      <c r="R5" s="4"/>
+      <c r="S5" s="14"/>
+      <c r="T5" s="14"/>
+      <c r="U5" s="14"/>
+    </row>
+    <row r="6" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B6" s="4">
+        <v>4</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
-      <c r="N5" s="6"/>
-    </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B6" s="6">
-        <v>4</v>
-      </c>
-      <c r="C6" s="6" t="s">
+      <c r="D6" s="19">
+        <v>44862</v>
+      </c>
+      <c r="E6" s="19">
+        <v>44868</v>
+      </c>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="14"/>
+      <c r="N6" s="4"/>
+      <c r="O6" s="4"/>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="4"/>
+      <c r="R6" s="4"/>
+      <c r="S6" s="14"/>
+      <c r="T6" s="14"/>
+      <c r="U6" s="14"/>
+    </row>
+    <row r="7" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B7" s="4">
+        <v>5</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="19">
+        <v>44862</v>
+      </c>
+      <c r="E7" s="19">
+        <v>44865</v>
+      </c>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="14"/>
+      <c r="N7" s="4"/>
+      <c r="O7" s="4"/>
+      <c r="P7" s="4"/>
+      <c r="Q7" s="4"/>
+      <c r="R7" s="4"/>
+      <c r="S7" s="14"/>
+      <c r="T7" s="14"/>
+      <c r="U7" s="14"/>
+    </row>
+    <row r="8" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B8" s="4">
+        <v>6</v>
+      </c>
+      <c r="C8" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6"/>
-      <c r="M6" s="6"/>
-      <c r="N6" s="6"/>
-    </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B7" s="6">
-        <v>5</v>
-      </c>
-      <c r="C7" s="7" t="s">
+      <c r="D8" s="19">
+        <v>44868</v>
+      </c>
+      <c r="E8" s="19">
+        <v>44872</v>
+      </c>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="15"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="4"/>
+      <c r="P8" s="4"/>
+      <c r="Q8" s="4"/>
+      <c r="R8" s="4"/>
+      <c r="S8" s="14"/>
+      <c r="T8" s="14"/>
+      <c r="U8" s="14"/>
+    </row>
+    <row r="9" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B9" s="4">
+        <v>7</v>
+      </c>
+      <c r="C9" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6"/>
-      <c r="M7" s="6"/>
-      <c r="N7" s="6"/>
-    </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B8" s="6">
-        <v>6</v>
-      </c>
-      <c r="C8" s="8" t="s">
+      <c r="D9" s="19">
+        <v>44865</v>
+      </c>
+      <c r="E9" s="19">
+        <v>44876</v>
+      </c>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="15"/>
+      <c r="M9" s="15"/>
+      <c r="N9" s="15"/>
+      <c r="O9" s="15"/>
+      <c r="P9" s="4"/>
+      <c r="Q9" s="4"/>
+      <c r="R9" s="4"/>
+      <c r="S9" s="14"/>
+      <c r="T9" s="14"/>
+      <c r="U9" s="14"/>
+    </row>
+    <row r="10" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B10" s="4">
+        <v>8</v>
+      </c>
+      <c r="C10" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="6"/>
-      <c r="M8" s="6"/>
-      <c r="N8" s="6"/>
-    </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B9" s="6">
-        <v>7</v>
-      </c>
-      <c r="C9" s="9" t="s">
+      <c r="D10" s="19">
+        <v>44872</v>
+      </c>
+      <c r="E10" s="19">
+        <v>44879</v>
+      </c>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="14"/>
+      <c r="L10" s="14"/>
+      <c r="M10" s="15"/>
+      <c r="N10" s="15"/>
+      <c r="O10" s="15"/>
+      <c r="P10" s="15"/>
+      <c r="Q10" s="4"/>
+      <c r="R10" s="4"/>
+      <c r="S10" s="14"/>
+      <c r="T10" s="14"/>
+      <c r="U10" s="14"/>
+    </row>
+    <row r="11" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B11" s="4">
+        <v>9</v>
+      </c>
+      <c r="C11" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="6"/>
-      <c r="M9" s="6"/>
-      <c r="N9" s="6"/>
-    </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B10" s="6">
-        <v>8</v>
-      </c>
-      <c r="C10" s="10" t="s">
+      <c r="D11" s="19">
+        <v>44872</v>
+      </c>
+      <c r="E11" s="19">
+        <v>44879</v>
+      </c>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="15"/>
+      <c r="N11" s="15"/>
+      <c r="O11" s="15"/>
+      <c r="P11" s="15"/>
+      <c r="Q11" s="4"/>
+      <c r="R11" s="4"/>
+      <c r="S11" s="14"/>
+      <c r="T11" s="14"/>
+      <c r="U11" s="14"/>
+    </row>
+    <row r="12" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B12" s="4">
+        <v>10</v>
+      </c>
+      <c r="C12" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
-      <c r="M10" s="6"/>
-      <c r="N10" s="6"/>
-    </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B11" s="6">
-        <v>9</v>
-      </c>
-      <c r="C11" s="11" t="s">
+      <c r="D12" s="19">
+        <v>44879</v>
+      </c>
+      <c r="E12" s="19">
+        <v>44883</v>
+      </c>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="14"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="14"/>
+      <c r="N12" s="4"/>
+      <c r="O12" s="4"/>
+      <c r="P12" s="15"/>
+      <c r="Q12" s="15"/>
+      <c r="R12" s="15"/>
+      <c r="S12" s="14"/>
+      <c r="T12" s="14"/>
+      <c r="U12" s="14"/>
+    </row>
+    <row r="13" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B13" s="4">
+        <v>11</v>
+      </c>
+      <c r="C13" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="6"/>
-      <c r="M11" s="6"/>
-      <c r="N11" s="6"/>
-    </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B12" s="6">
-        <v>10</v>
-      </c>
-      <c r="C12" s="12" t="s">
+      <c r="D13" s="19">
+        <v>44883</v>
+      </c>
+      <c r="E13" s="19">
+        <v>44886</v>
+      </c>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="14"/>
+      <c r="L13" s="14"/>
+      <c r="M13" s="14"/>
+      <c r="N13" s="4"/>
+      <c r="O13" s="4"/>
+      <c r="P13" s="4"/>
+      <c r="Q13" s="4"/>
+      <c r="R13" s="15"/>
+      <c r="S13" s="15"/>
+      <c r="T13" s="14"/>
+      <c r="U13" s="14"/>
+    </row>
+    <row r="14" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B14" s="4">
+        <v>12</v>
+      </c>
+      <c r="C14" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="6"/>
-      <c r="M12" s="6"/>
-      <c r="N12" s="6"/>
-    </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B13" s="6">
-        <v>11</v>
-      </c>
-      <c r="C13" s="13" t="s">
+      <c r="D14" s="19">
+        <v>44886</v>
+      </c>
+      <c r="E14" s="19">
+        <v>44889</v>
+      </c>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="14"/>
+      <c r="L14" s="14"/>
+      <c r="M14" s="14"/>
+      <c r="N14" s="4"/>
+      <c r="O14" s="4"/>
+      <c r="P14" s="4"/>
+      <c r="Q14" s="4"/>
+      <c r="R14" s="4"/>
+      <c r="S14" s="15"/>
+      <c r="T14" s="15"/>
+      <c r="U14" s="14"/>
+    </row>
+    <row r="15" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B15" s="4">
+        <v>13</v>
+      </c>
+      <c r="C15" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
-      <c r="K13" s="6"/>
-      <c r="L13" s="6"/>
-      <c r="M13" s="6"/>
-      <c r="N13" s="6"/>
-    </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B14" s="6">
-        <v>12</v>
-      </c>
-      <c r="C14" s="14" t="s">
+      <c r="D15" s="19">
+        <v>44889</v>
+      </c>
+      <c r="E15" s="19">
+        <v>44890</v>
+      </c>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="14"/>
+      <c r="M15" s="14"/>
+      <c r="N15" s="4"/>
+      <c r="O15" s="4"/>
+      <c r="P15" s="4"/>
+      <c r="Q15" s="4"/>
+      <c r="R15" s="4"/>
+      <c r="S15" s="14"/>
+      <c r="T15" s="15"/>
+      <c r="U15" s="15"/>
+    </row>
+    <row r="16" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B16" s="4">
+        <v>14</v>
+      </c>
+      <c r="C16" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
-      <c r="K14" s="6"/>
-      <c r="L14" s="6"/>
-      <c r="M14" s="6"/>
-      <c r="N14" s="6"/>
-    </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B15" s="6">
-        <v>13</v>
-      </c>
-      <c r="C15" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="6"/>
-      <c r="K15" s="6"/>
-      <c r="L15" s="6"/>
-      <c r="M15" s="6"/>
-      <c r="N15" s="6"/>
-    </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B16" s="6">
-        <v>14</v>
-      </c>
-      <c r="C16" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="6"/>
-      <c r="K16" s="6"/>
-      <c r="L16" s="6"/>
-      <c r="M16" s="6"/>
-      <c r="N16" s="6"/>
-    </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B17" s="6">
+      <c r="D16" s="19">
+        <v>44855</v>
+      </c>
+      <c r="E16" s="19">
+        <v>44890</v>
+      </c>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="15"/>
+      <c r="J16" s="15"/>
+      <c r="K16" s="15"/>
+      <c r="L16" s="15"/>
+      <c r="M16" s="15"/>
+      <c r="N16" s="15"/>
+      <c r="O16" s="15"/>
+      <c r="P16" s="15"/>
+      <c r="Q16" s="15"/>
+      <c r="R16" s="15"/>
+      <c r="S16" s="15"/>
+      <c r="T16" s="15"/>
+      <c r="U16" s="15"/>
+    </row>
+    <row r="17" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B17" s="4">
         <v>15</v>
       </c>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="6"/>
-      <c r="K17" s="6"/>
-      <c r="L17" s="6"/>
-      <c r="M17" s="6"/>
-      <c r="N17" s="6"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="14"/>
+      <c r="L17" s="14"/>
+      <c r="M17" s="14"/>
+      <c r="N17" s="4"/>
+      <c r="O17" s="4"/>
+      <c r="P17" s="4"/>
+      <c r="Q17" s="4"/>
+      <c r="R17" s="4"/>
+      <c r="S17" s="14"/>
+      <c r="T17" s="14"/>
+      <c r="U17" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>